<commit_message>
1: ma cross with ml prediction
</commit_message>
<xml_diff>
--- a/machine_logs/test_rsi.xlsx
+++ b/machine_logs/test_rsi.xlsx
@@ -542,7 +542,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -725,6 +725,132 @@
         <v>0</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-09-06</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>76796000</v>
+      </c>
+      <c r="C9" t="n">
+        <v>30.54235498227352</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-09-06</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>76796000</v>
+      </c>
+      <c r="C10" t="n">
+        <v>30.54235498227352</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-09-06</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>76796000</v>
+      </c>
+      <c r="C11" t="n">
+        <v>30.54235498227352</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-09-11</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>77938000</v>
+      </c>
+      <c r="C12" t="n">
+        <v>31.95390905711808</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" t="n">
+        <v>77938000</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-09-11</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>77938000</v>
+      </c>
+      <c r="C13" t="n">
+        <v>31.95390905711808</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" t="n">
+        <v>77938000</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>86259000</v>
+      </c>
+      <c r="C14" t="n">
+        <v>69.91787829833063</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>86702330</v>
+      </c>
+      <c r="H14" t="n">
+        <v>87001000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>